<commit_message>
multigraphgit add .git add .
</commit_message>
<xml_diff>
--- a/xls/subject_data_visualizations.xlsx
+++ b/xls/subject_data_visualizations.xlsx
@@ -280,7 +280,7 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$A$5:$A$10</c:f>
+              <c:f>(Sheet1!$A$5:$A$8,Sheet1!$A$10:$A$11)</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -296,10 +296,10 @@
                   <c:v>1900-1999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2000-2099</c:v>
+                  <c:v>No Period Listed</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>No Period Listed</c:v>
+                  <c:v>Total</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -313,7 +313,7 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$B$5:$B$10</c:f>
+              <c:f>(Sheet1!$B$5:$B$8,Sheet1!$B$10:$B$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -330,10 +330,271 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coverage of literature by century in 1950</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>1600-1699</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1700-1799</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>1800-1899</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1900-1999</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>No Period Listed</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Total</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$22:$B$28</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$22:$B$25,Sheet1!$B$27:$B$28)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coverage of literature by century in 1980</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>1600-1699</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1700-1799</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>1800-1899</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1900-1999</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>No Period Listed</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Total</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$37:$B$43</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$37:$B$40,Sheet1!$B$42:$B$43)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$52</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coverage of literature by century in 2010</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>1600-1699</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1700-1799</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>1800-1899</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1900-1999</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>No Period Listed</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Total</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$53:$B$59</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$B$53:$B$56,Sheet1!$B$58:$B$59)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -349,122 +610,12 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="235508608"/>
-        <c:axId val="235503568"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredBarSeries>
-              <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$C$2:$C$4</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="3"/>
-                      <c:pt idx="0">
-                        <c:v>All data</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>% of articles</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:invertIfNegative val="0"/>
-                <c:cat>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:fullRef>
-                          <c15:sqref>Sheet1!$A$5:$A$11</c15:sqref>
-                        </c15:fullRef>
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$5:$A$10</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="6"/>
-                      <c:pt idx="0">
-                        <c:v>1600-1699</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>1700-1799</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>1800-1899</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>1900-1999</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>2000-2099</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>No Period Listed</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:fullRef>
-                          <c15:sqref>Sheet1!$C$5:$C$11</c15:sqref>
-                        </c15:fullRef>
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$C$5:$C$10</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0%</c:formatCode>
-                      <c:ptCount val="6"/>
-                      <c:pt idx="0">
-                        <c:v>3.0927835051546393E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>5.1546391752577317E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0.60824742268041232</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0.27835051546391754</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>3.0927835051546393E-2</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-              </c15:ser>
-            </c15:filteredBarSeries>
-          </c:ext>
-        </c:extLst>
+        <c:axId val="264567424"/>
+        <c:axId val="264570224"/>
+        <c:extLst/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="235508608"/>
+        <c:axId val="264567424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -507,7 +658,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235503568"/>
+        <c:crossAx val="264570224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -515,9 +666,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235503568"/>
+        <c:axId val="264570224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -566,7 +718,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235508608"/>
+        <c:crossAx val="264567424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -834,8 +986,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="240954592"/>
-        <c:axId val="240957952"/>
+        <c:axId val="265977504"/>
+        <c:axId val="265978064"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -949,7 +1101,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="240954592"/>
+        <c:axId val="265977504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -992,7 +1144,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240957952"/>
+        <c:crossAx val="265978064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1000,7 +1152,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="240957952"/>
+        <c:axId val="265978064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1051,7 +1203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240954592"/>
+        <c:crossAx val="265977504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1311,8 +1463,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="242778768"/>
-        <c:axId val="242777648"/>
+        <c:axId val="265981424"/>
+        <c:axId val="265981984"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1423,7 +1575,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="242778768"/>
+        <c:axId val="265981424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1466,7 +1618,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242777648"/>
+        <c:crossAx val="265981984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1474,7 +1626,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242777648"/>
+        <c:axId val="265981984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1525,7 +1677,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242778768"/>
+        <c:crossAx val="265981424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1808,8 +1960,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="238358976"/>
-        <c:axId val="330637008"/>
+        <c:axId val="267092752"/>
+        <c:axId val="267093312"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1920,7 +2072,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="238358976"/>
+        <c:axId val="267092752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1963,7 +2115,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330637008"/>
+        <c:crossAx val="267093312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1971,7 +2123,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="330637008"/>
+        <c:axId val="267093312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2022,7 +2174,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238358976"/>
+        <c:crossAx val="267092752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4666,7 +4818,7 @@
   <dimension ref="A2:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N49" sqref="N49"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>